<commit_message>
Base Organization became Identified Organization
DR-77
Design approach agreed within CI:

Scenarios often require a name or an id or both
Attempt to support the scenarios by developing a reusable profile
The scenario constraint will be set in the profile that references this e.g. if an order requester then name is mandatory (the rule is in the order profile)
Current working title of these profiles is "Identified x" as the usage scenario calls for some meaningful identication (cannot be an unknown entity)
</commit_message>
<xml_diff>
--- a/output/DiagnosticReport/patient-ident-1.xlsx
+++ b/output/DiagnosticReport/patient-ident-1.xlsx
@@ -1049,7 +1049,7 @@
     <t>Patient.contact.organization</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/organization-dh-base-1)
+    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/organization-identified-1)
 </t>
   </si>
   <si>
@@ -1176,7 +1176,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/organization-dh-base-1|http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/practitionerrole-dh-base-1)
+    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/organization-identified-1|http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/practitionerrole-dh-base-1)
 </t>
   </si>
   <si>

</xml_diff>

<commit_message>
Regenerated the outputs after the changes performed on Patient with Mandatory Identifier (patient-ident-1) profile
DR-48
</commit_message>
<xml_diff>
--- a/output/DiagnosticReport/patient-ident-1.xlsx
+++ b/output/DiagnosticReport/patient-ident-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2354" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2354" uniqueCount="402">
   <si>
     <t>Path</t>
   </si>
@@ -160,7 +160,7 @@
   </si>
   <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}inv-pat-0:If there is a birth time its date shall be the birth date {birthDate.extension('http://hl7.org/fhir/StructureDefinition/patient-birthTime').exists() implies birthDate.extension('http://hl7.org/fhir/StructureDefinition/patient-birthTime').value.toString().substring(0,10) = birthDate.toString()}inv-dh-pat-01:If present, a general practitioner shall at least have a reference, an identifier or a display {generalPractitioner.exists() implies generalPractitioner.all($this.reference.exists() or $this.identifier.exists() or $this.display.exists())}inv-dh-pat-02:If present, a managing organisation shall at least have a reference, an identifier or a display {managingOrganization.exists() implies (managingOrganization.reference.exists() or managingOrganization.identifier.exists() or managingOrganization.display.exists())}inv-dh-pat-03:At least one patient identifier shall at least have a system and a value {identifier.where(system.count() + value.count() &gt;1).exists()}inv-dh-pat-04:If present, date of arrival shall be year of arrival {extension('http://hl7.org.au/fhir/StructureDefinition/date-of-arrival').exists() implies extension.valueDate.value.matches('^([0-9]{4})$')}</t>
+dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}inv-pat-0:If there is a birth time its date shall be the birth date {birthDate.extension('http://hl7.org/fhir/StructureDefinition/patient-birthTime').exists() implies birthDate.extension('http://hl7.org/fhir/StructureDefinition/patient-birthTime').value.toString().substring(0,10) = birthDate.toString()}inv-dh-pat-01:If present, a general practitioner shall at least have a reference, an identifier or a display {generalPractitioner.exists() implies generalPractitioner.all($this.reference.exists() or $this.identifier.exists() or $this.display.exists())}inv-dh-pat-02:At least one patient identifier shall at least have a system and a value {identifier.where(system.count() + value.count() &gt;1).exists()}inv-dh-pat-03:If present, date of arrival shall be year of arrival {extension('http://hl7.org.au/fhir/StructureDefinition/date-of-arrival').exists() implies extension.valueDate.value.matches('^([0-9]{4})$')}</t>
   </si>
   <si>
     <t>Patient[classCode=PAT]</t>
@@ -926,7 +926,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-pat-1:SHALL at least contain a contact's details or a reference to an organization {name.exists() or telecom.exists() or address.exists() or organization.exists()}inv-dh-pat-05:If present, a contact's organisation shall at least have a reference, an identifier or a display {organization.exists() implies (organization.reference.exists() or organization.identifier.exists() or organization.display.exists())}</t>
+pat-1:SHALL at least contain a contact's details or a reference to an organization {name.exists() or telecom.exists() or address.exists() or organization.exists()}inv-dh-pat-04:If present, a contact's organisation shall at least have a reference, an identifier or a display {organization.exists() implies (organization.reference.exists() or organization.identifier.exists() or organization.display.exists())}</t>
   </si>
   <si>
     <t>player[classCode=PSN|ANM and determinerCode=INSTANCE]/scopedRole[classCode=CON]</t>
@@ -1198,6 +1198,10 @@
   </si>
   <si>
     <t>Patient.managingOrganization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference(Organization)
+</t>
   </si>
   <si>
     <t>Organization that is the custodian of the patient record</t>
@@ -2732,7 +2736,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
         <v>95</v>
       </c>
@@ -2750,7 +2754,7 @@
         <v>51</v>
       </c>
       <c r="G12" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="H12" t="s" s="2">
         <v>44</v>
@@ -8116,7 +8120,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
         <v>374</v>
       </c>
@@ -8132,7 +8136,7 @@
         <v>51</v>
       </c>
       <c r="G59" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="H59" t="s" s="2">
         <v>44</v>
@@ -8141,19 +8145,19 @@
         <v>52</v>
       </c>
       <c r="J59" t="s" s="2">
-        <v>327</v>
+        <v>375</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="N59" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="O59" t="s" s="2">
         <v>44</v>
@@ -8220,7 +8224,7 @@
         <v>332</v>
       </c>
       <c r="AK59" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="AL59" t="s" s="2">
         <v>44</v>
@@ -8234,7 +8238,7 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
@@ -8260,16 +8264,16 @@
         <v>282</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="M60" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="N60" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="O60" t="s" s="2">
         <v>44</v>
@@ -8318,7 +8322,7 @@
         <v>44</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>42</v>
@@ -8333,7 +8337,7 @@
         <v>63</v>
       </c>
       <c r="AJ60" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="AK60" t="s" s="2">
         <v>163</v>
@@ -8350,7 +8354,7 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -8462,7 +8466,7 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -8576,7 +8580,7 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -8692,7 +8696,7 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
@@ -8715,16 +8719,16 @@
         <v>52</v>
       </c>
       <c r="J64" t="s" s="2">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="K64" t="s" s="2">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="M64" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="N64" s="2"/>
       <c r="O64" t="s" s="2">
@@ -8774,7 +8778,7 @@
         <v>44</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="AF64" t="s" s="2">
         <v>51</v>
@@ -8789,7 +8793,7 @@
         <v>63</v>
       </c>
       <c r="AJ64" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="AK64" t="s" s="2">
         <v>163</v>
@@ -8798,7 +8802,7 @@
         <v>44</v>
       </c>
       <c r="AM64" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="AN64" t="s" s="2">
         <v>44</v>
@@ -8806,7 +8810,7 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
@@ -8832,10 +8836,10 @@
         <v>71</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="M65" s="2"/>
       <c r="N65" s="2"/>
@@ -8865,10 +8869,10 @@
         <v>188</v>
       </c>
       <c r="X65" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="Y65" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="Z65" t="s" s="2">
         <v>44</v>
@@ -8886,7 +8890,7 @@
         <v>44</v>
       </c>
       <c r="AE65" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="AF65" t="s" s="2">
         <v>51</v>
@@ -8901,7 +8905,7 @@
         <v>63</v>
       </c>
       <c r="AJ65" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="AK65" t="s" s="2">
         <v>163</v>

</xml_diff>